<commit_message>
add BOM3 changes and smaller CAD version
</commit_message>
<xml_diff>
--- a/HyperRail_BOMv3.xlsx
+++ b/HyperRail_BOMv3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Brusind\Documents\GitHub\HyperRail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151F8590-5926-490B-B1F0-37C306A63AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0754E01-B843-409F-81BE-47600DE363B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="3" xr2:uid="{9AA5CA3B-103F-4503-BB38-84DF181EF15E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" xr2:uid="{9AA5CA3B-103F-4503-BB38-84DF181EF15E}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="445">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -414,9 +414,6 @@
     <t>DIODE SCHOTTKY 20V 500MA SOD123</t>
   </si>
   <si>
-    <t>Integrated Stepper Driver PCB</t>
-  </si>
-  <si>
     <t>3_3V, 5V, 24V</t>
   </si>
   <si>
@@ -724,9 +721,6 @@
   </si>
   <si>
     <t>Category</t>
-  </si>
-  <si>
-    <t>Main Electrical System Assembly</t>
   </si>
   <si>
     <t>Mechanical</t>
@@ -10290,8 +10284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2C5D0B-A61F-416F-933C-0297DCE53E09}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10315,7 +10309,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="33.75">
       <c r="A1" s="38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -10330,7 +10324,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>3</v>
@@ -10351,19 +10345,19 @@
         <v>11</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L2" s="28">
         <f>SUM(Table13[Extended Price])</f>
-        <v>1583.4433625459321</v>
+        <v>1408.0033625459321</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="C3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -10377,12 +10371,12 @@
         <v>896.49961921259842</v>
       </c>
       <c r="I3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="18" thickBot="1">
       <c r="C4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -10396,79 +10390,55 @@
         <v>261.02616</v>
       </c>
       <c r="I4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K4" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L4" s="30"/>
     </row>
     <row r="5" spans="1:18" ht="27" thickTop="1">
-      <c r="C5" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="I5" t="s">
         <v>226</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7">
-        <f>'Electrical '!I60</f>
-        <v>105.52000000000001</v>
-      </c>
-      <c r="F5" s="7">
-        <f>Table13[[#This Row],[Unit Price]]*Table13[[#This Row],[Quantity]]</f>
-        <v>105.52000000000001</v>
-      </c>
-      <c r="I5" t="s">
-        <v>228</v>
-      </c>
       <c r="K5" s="39" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L5" s="39"/>
       <c r="M5" s="39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="N5" s="39"/>
       <c r="P5" s="29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="R5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="C6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="7">
-        <f>'Electrical '!I24</f>
-        <v>17.48</v>
-      </c>
-      <c r="F6" s="7">
-        <f>Table13[[#This Row],[Unit Price]]*Table13[[#This Row],[Quantity]]</f>
-        <v>69.92</v>
-      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
       <c r="I6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L6" s="25">
         <v>1.5</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="N6" s="25">
         <f>L6</f>
         <v>1.5</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Q6">
         <f>N6*(N9+1)</f>
@@ -10481,7 +10451,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="C7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -10495,23 +10465,23 @@
         <v>34.43</v>
       </c>
       <c r="I7" t="s">
+        <v>226</v>
+      </c>
+      <c r="K7" s="24" t="s">
         <v>228</v>
-      </c>
-      <c r="K7" s="24" t="s">
-        <v>230</v>
       </c>
       <c r="L7" s="25">
         <v>2</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="N7" s="25">
         <f t="shared" ref="N7:N8" si="0">L7</f>
         <v>2</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="Q7">
         <f>N7*(N9+1)</f>
@@ -10524,7 +10494,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="C8" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -10538,20 +10508,20 @@
         <v>216.04758333333342</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L8" s="25">
         <v>2</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="N8" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="Q8">
         <f>N8*(N9+1)</f>
@@ -10566,7 +10536,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="M9" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -10668,7 +10638,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -10703,19 +10673,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -10727,27 +10697,27 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="34">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -10762,13 +10732,13 @@
         <v>0.51273000000000002</v>
       </c>
       <c r="H3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K3" s="32" t="str">
         <f>HYPERLINK("https://www.amazon.com/Aluminum-Extrusion-European-Standard-Anodized/dp/B08CN92SP1/ref=sr_1_7?crid=3VIGODRUEW0NZ&amp;keywords=150mm+2040&amp;qid=1645476496&amp;sprefix=150mm+2040%2Caps%2C147&amp;sr=8-7", "Amazon")</f>
@@ -10781,13 +10751,13 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="34" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C4" s="31">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E4" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3pcU6xT", "Amazon")</f>
@@ -10802,19 +10772,19 @@
         <v>3.198</v>
       </c>
       <c r="H4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C5" s="34">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -10829,22 +10799,22 @@
         <v>0.30384</v>
       </c>
       <c r="H5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C6" s="34">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E6" s="32" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/970300581/6174852", "DigiKey")</f>
@@ -10858,7 +10828,7 @@
         <v>0.76</v>
       </c>
       <c r="H6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K6" s="32" t="str">
         <f t="shared" ref="K6" si="0">HYPERLINK("", "Amazon")</f>
@@ -10867,13 +10837,13 @@
     </row>
     <row r="7" spans="1:32" ht="50.1" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C7" s="34">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E7" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A218/", "McMaster")</f>
@@ -10888,10 +10858,10 @@
         <v>0.73760000000000003</v>
       </c>
       <c r="H7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K7" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3I2Pemt", "Amazon")</f>
@@ -10900,13 +10870,13 @@
     </row>
     <row r="8" spans="1:32" ht="50.1" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C8" s="34">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E8" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A223/", "McMaster")</f>
@@ -10921,10 +10891,10 @@
         <v>1.7775999999999998</v>
       </c>
       <c r="H8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K8" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3sVaTGL", "Amazon")</f>
@@ -10933,13 +10903,13 @@
     </row>
     <row r="9" spans="1:32" ht="50.1" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C9" s="34">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E9" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90591A260/", "McMaster")</f>
@@ -10954,10 +10924,10 @@
         <v>7.1199999999999999E-2</v>
       </c>
       <c r="H9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K9" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3v5pm5K", "Amazon")</f>
@@ -11479,7 +11449,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -11514,19 +11484,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -11538,27 +11508,27 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="31" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="31">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -11573,7 +11543,7 @@
         <v>0.51273000000000002</v>
       </c>
       <c r="H3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="7">
@@ -11583,13 +11553,13 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="31" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C4" s="31">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E4" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3pcU6xT", "Amazon")</f>
@@ -11604,19 +11574,19 @@
         <v>1.599</v>
       </c>
       <c r="H4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="31" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C5" s="31">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -11631,22 +11601,22 @@
         <v>0.30384</v>
       </c>
       <c r="H5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C6" s="31">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E6" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3t3zuJQ", "F606ZZ")</f>
@@ -11664,13 +11634,13 @@
     </row>
     <row r="7" spans="1:32" ht="50.1" customHeight="1">
       <c r="A7" s="31" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C7" s="31">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -11685,19 +11655,19 @@
         <v>0.22788</v>
       </c>
       <c r="H7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:32" ht="50.1" customHeight="1">
       <c r="A8" s="31" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C8" s="31">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E8" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A223/", "McMaster")</f>
@@ -11712,10 +11682,10 @@
         <v>1.7775999999999998</v>
       </c>
       <c r="H8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K8" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3sVaTGL", "Amazon")</f>
@@ -12305,7 +12275,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -12340,19 +12310,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -12364,27 +12334,27 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C3" s="34">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" s="32" t="str">
         <f t="shared" ref="E3" si="0">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -12399,10 +12369,10 @@
         <v>0.37980000000000003</v>
       </c>
       <c r="H3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="7">
@@ -12412,13 +12382,13 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="34" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C4" s="34">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E4" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -12433,22 +12403,22 @@
         <v>0.15192</v>
       </c>
       <c r="H4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="34" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C5" s="34">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3t3zuJQ", "F606ZZ")</f>
@@ -12466,13 +12436,13 @@
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C6" s="34">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E6" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A223/", "McMaster")</f>
@@ -12487,10 +12457,10 @@
         <v>0.88879999999999992</v>
       </c>
       <c r="H6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K6" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3sVaTGL", "Amazon")</f>
@@ -12608,7 +12578,7 @@
     </row>
     <row r="22" spans="1:11" ht="50.1" customHeight="1">
       <c r="A22" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -13041,7 +13011,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -13076,19 +13046,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -13100,27 +13070,27 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="31" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C3" s="31">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" s="32" t="str">
         <f t="shared" ref="E3" si="0">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -13135,7 +13105,7 @@
         <v>0.41777999999999998</v>
       </c>
       <c r="H3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="7">
@@ -13145,13 +13115,13 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="31" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C4" s="31">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E4" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -13166,19 +13136,19 @@
         <v>0.13292999999999999</v>
       </c>
       <c r="H4" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="34" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C5" s="31">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E5" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/62805K49/", "McMaster")</f>
@@ -13192,19 +13162,19 @@
         <v>5.72</v>
       </c>
       <c r="H5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C6" s="31">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E6" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A222/", "McMaster")</f>
@@ -13219,13 +13189,13 @@
         <v>0.53239999999999998</v>
       </c>
       <c r="H6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K6" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/35ijWtt", "Amazon")</f>
@@ -13234,13 +13204,13 @@
     </row>
     <row r="7" spans="1:32" ht="50.1" customHeight="1">
       <c r="A7" s="31" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C7" s="31">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E7" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90592A016/","McMaster")</f>
@@ -13255,13 +13225,13 @@
         <v>6.2400000000000004E-2</v>
       </c>
       <c r="H7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K7" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3JKgFBP","Amazon")</f>
@@ -13371,7 +13341,7 @@
     </row>
     <row r="22" spans="1:11" ht="50.1" customHeight="1">
       <c r="A22" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -13791,7 +13761,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="58.5" customHeight="1">
       <c r="A1" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -13855,7 +13825,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -14563,7 +14533,7 @@
         <v>32</v>
       </c>
       <c r="P17" s="36" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -14718,7 +14688,7 @@
     </row>
     <row r="24" spans="1:16" ht="27.75" customHeight="1">
       <c r="A24" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B24" s="40"/>
       <c r="C24" s="40"/>
@@ -14734,7 +14704,7 @@
     </row>
     <row r="25" spans="1:16" ht="47.25" customHeight="1">
       <c r="A25" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="42"/>
@@ -14809,7 +14779,7 @@
         <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>19</v>
@@ -14847,16 +14817,16 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>51</v>
@@ -14880,7 +14850,7 @@
         <v>41</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>23</v>
@@ -14894,16 +14864,16 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>19</v>
@@ -14924,10 +14894,10 @@
         <v>936348</v>
       </c>
       <c r="K29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L29" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>23</v>
@@ -14941,16 +14911,16 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>19</v>
@@ -14974,7 +14944,7 @@
         <v>30</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>23</v>
@@ -14997,7 +14967,7 @@
         <v>28</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>19</v>
@@ -15035,16 +15005,16 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>19</v>
@@ -15065,10 +15035,10 @@
         <v>78973</v>
       </c>
       <c r="K32" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>23</v>
@@ -15091,7 +15061,7 @@
         <v>49</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>51</v>
@@ -15129,16 +15099,16 @@
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>51</v>
@@ -15162,7 +15132,7 @@
         <v>52</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>23</v>
@@ -15179,13 +15149,13 @@
         <v>5040771891</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>19</v>
@@ -15206,10 +15176,10 @@
         <v>2400</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>23</v>
@@ -15223,16 +15193,16 @@
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>19</v>
@@ -15256,7 +15226,7 @@
         <v>115</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>25</v>
@@ -15270,16 +15240,16 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>19</v>
@@ -15300,10 +15270,10 @@
         <v>246</v>
       </c>
       <c r="K37" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L37" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>23</v>
@@ -15317,16 +15287,16 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>19</v>
@@ -15347,10 +15317,10 @@
         <v>24018</v>
       </c>
       <c r="K38" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>23</v>
@@ -15373,7 +15343,7 @@
         <v>83</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>19</v>
@@ -15420,7 +15390,7 @@
         <v>88</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>19</v>
@@ -15458,16 +15428,16 @@
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>19</v>
@@ -15491,7 +15461,7 @@
         <v>21</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>23</v>
@@ -15505,16 +15475,16 @@
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>51</v>
@@ -15535,10 +15505,10 @@
         <v>67015</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>54</v>
@@ -15552,16 +15522,16 @@
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>19</v>
@@ -15582,10 +15552,10 @@
         <v>0</v>
       </c>
       <c r="K43" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>23</v>
@@ -15608,7 +15578,7 @@
         <v>113</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>19</v>
@@ -15646,16 +15616,16 @@
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>96</v>
@@ -15679,7 +15649,7 @@
         <v>109</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>23</v>
@@ -15693,16 +15663,16 @@
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>112</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>19</v>
@@ -15726,7 +15696,7 @@
         <v>109</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M46" s="2" t="s">
         <v>23</v>
@@ -15749,7 +15719,7 @@
         <v>119</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>19</v>
@@ -15787,22 +15757,22 @@
     </row>
     <row r="48" spans="1:15" ht="16.5" customHeight="1">
       <c r="A48" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G48" s="2">
         <v>1</v>
@@ -15820,7 +15790,7 @@
         <v>21</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M48" s="2" t="s">
         <v>23</v>
@@ -15885,7 +15855,7 @@
     </row>
     <row r="52" spans="1:15" ht="27.75" customHeight="1">
       <c r="A52" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B52" s="40"/>
       <c r="C52" s="40"/>
@@ -15901,7 +15871,7 @@
     </row>
     <row r="53" spans="1:15" ht="41.25" customHeight="1">
       <c r="A53" s="43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
@@ -15967,16 +15937,16 @@
     </row>
     <row r="55" spans="1:15">
       <c r="A55" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="C55" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>210</v>
-      </c>
       <c r="D55" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>51</v>
@@ -16000,7 +15970,7 @@
         <v>58</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M55" s="8" t="s">
         <v>54</v>
@@ -16014,17 +15984,17 @@
     </row>
     <row r="56" spans="1:15">
       <c r="A56" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>212</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>213</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>20</v>
@@ -16044,7 +16014,7 @@
       </c>
       <c r="K56" s="8"/>
       <c r="L56" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M56" s="8" t="s">
         <v>23</v>
@@ -16109,7 +16079,7 @@
     </row>
     <row r="60" spans="1:15" ht="27.75" customHeight="1">
       <c r="A60" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B60" s="40"/>
       <c r="C60" s="40"/>
@@ -16260,7 +16230,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -16295,19 +16265,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -16319,27 +16289,27 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C3" s="31">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E3" s="32" t="str">
         <f>HYPERLINK("https://bit.ly/3vasq0u", "StepperOnline")</f>
@@ -16353,10 +16323,10 @@
         <v>54.77</v>
       </c>
       <c r="H3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="7">
@@ -16366,13 +16336,13 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="31" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C4" s="31">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E4" s="32"/>
       <c r="F4" s="5">
@@ -16383,22 +16353,22 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="31" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C5" s="31">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="5">
@@ -16410,16 +16380,16 @@
         <v>17.48</v>
       </c>
       <c r="H5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C6" s="31">
         <v>1</v>
@@ -16440,22 +16410,22 @@
         <v>53.691102362204731</v>
       </c>
       <c r="H6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:32" ht="50.1" customHeight="1">
       <c r="A7" s="31" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C7" s="31">
         <v>1</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="32" t="str">
         <f t="shared" ref="E7" si="0">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -16470,23 +16440,23 @@
         <v>1.55718</v>
       </c>
       <c r="H7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:32" ht="50.1" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C8" s="31">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E8" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/98952A059/","McMaster")</f>
@@ -16503,13 +16473,13 @@
     </row>
     <row r="9" spans="1:32" ht="50.1" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C9" s="31">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E9" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/95783A039/","McMaster")</f>
@@ -16526,13 +16496,13 @@
     </row>
     <row r="10" spans="1:32" ht="50.1" customHeight="1">
       <c r="A10" s="34" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C10" s="31">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E10" s="32" t="str">
         <f>HYPERLINK("https://bit.ly/3Hc5Mr5","Misumi")</f>
@@ -16546,19 +16516,19 @@
         <v>46.32</v>
       </c>
       <c r="H10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K10" s="32"/>
     </row>
     <row r="11" spans="1:32" ht="50.1" customHeight="1">
       <c r="A11" s="31" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C11" s="31">
         <v>1</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E11" s="32" t="str">
         <f t="shared" ref="E11" si="1">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -16573,17 +16543,17 @@
         <v>0.15192</v>
       </c>
       <c r="H11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:32" ht="50.1" customHeight="1">
       <c r="A12" s="34" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C12" s="31">
         <v>1</v>
@@ -16606,13 +16576,13 @@
     </row>
     <row r="13" spans="1:32" ht="50.1" customHeight="1">
       <c r="A13" s="31" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C13" s="31">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E13" s="32" t="str">
         <f>HYPERLINK("https://www.amazon.com/gp/product/B07CXNK33Q/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1","Amazon")</f>
@@ -16626,22 +16596,22 @@
         <v>2.5</v>
       </c>
       <c r="H13" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:32" ht="50.1" customHeight="1">
       <c r="A14" s="31" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C14" s="31">
         <v>1</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E14" s="32" t="str">
         <f t="shared" ref="E14" si="2">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -16656,23 +16626,23 @@
         <v>0.34182000000000001</v>
       </c>
       <c r="H14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:32" ht="50.1" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C15" s="31">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E15" s="32" t="str">
         <f>HYPERLINK("https://shop.sdp-si.com/catalog/product/?id=A_6A55M028DF0912","SDPSI")</f>
@@ -16689,13 +16659,13 @@
     </row>
     <row r="16" spans="1:32" ht="50.1" customHeight="1">
       <c r="A16" s="34" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C16" s="31">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E16" s="32" t="str">
         <f>HYPERLINK("https://bit.ly/3BHYvxY","PolyBelt")</f>
@@ -16710,13 +16680,13 @@
         <v>20.497047244094492</v>
       </c>
       <c r="H16" t="s">
+        <v>347</v>
+      </c>
+      <c r="I16" t="s">
+        <v>348</v>
+      </c>
+      <c r="J16" t="s">
         <v>349</v>
-      </c>
-      <c r="I16" t="s">
-        <v>350</v>
-      </c>
-      <c r="J16" t="s">
-        <v>351</v>
       </c>
       <c r="K16" s="32" t="str">
         <f>HYPERLINK("https://www.ebay.com/itm/382865666347?var=651553605528","Ebay")</f>
@@ -16725,13 +16695,13 @@
     </row>
     <row r="17" spans="1:11" ht="50.1" customHeight="1">
       <c r="A17" s="31" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C17" s="31">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F17" s="35">
         <f>'Mechanical - Carriage Assembly'!L3</f>
@@ -16742,19 +16712,19 @@
         <v>107.97528</v>
       </c>
       <c r="H17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="50.1" customHeight="1">
       <c r="A18" s="31" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C18" s="31">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E18" s="32" t="str">
         <f>HYPERLINK("https://bit.ly/3payYID", "Stepper Online")</f>
@@ -16768,19 +16738,19 @@
         <v>1.84</v>
       </c>
       <c r="H18" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="50.1" customHeight="1">
       <c r="A19" s="31" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C19" s="31">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E19" s="32" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/littelfuse-inc/59145-040/4771993","Digikey")</f>
@@ -16794,19 +16764,19 @@
         <v>4.95</v>
       </c>
       <c r="H19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" ht="50.1" customHeight="1">
       <c r="A20" s="31" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C20" s="31">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E20" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/35hVTdS","Amazon")</f>
@@ -16820,19 +16790,19 @@
         <v>6.76</v>
       </c>
       <c r="H20" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="K20" s="32"/>
     </row>
     <row r="21" spans="1:11" ht="50.1" customHeight="1">
       <c r="A21" s="31" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C21" s="31">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E21" s="32" t="str">
         <f t="shared" ref="E21:E24" si="3">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -16847,23 +16817,23 @@
         <v>1.48122</v>
       </c>
       <c r="H21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
     <row r="22" spans="1:11" ht="50.1" customHeight="1">
       <c r="A22" s="31" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C22" s="31">
         <v>1</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E22" s="32" t="str">
         <f t="shared" si="3"/>
@@ -16878,23 +16848,23 @@
         <v>0.22788</v>
       </c>
       <c r="H22" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
     <row r="23" spans="1:11" ht="50.1" customHeight="1">
       <c r="A23" s="31" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C23" s="31">
         <v>1</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E23" s="32" t="str">
         <f t="shared" si="3"/>
@@ -16909,23 +16879,23 @@
         <v>0.20888999999999999</v>
       </c>
       <c r="H23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:11" ht="50.1" customHeight="1">
       <c r="A24" s="31" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C24" s="31">
         <v>1</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E24" s="32" t="str">
         <f t="shared" si="3"/>
@@ -16940,23 +16910,23 @@
         <v>0.30384</v>
       </c>
       <c r="H24" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" ht="50.1" customHeight="1">
       <c r="A25" s="31" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C25" s="31">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E25" s="32" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/littelfuse-inc/57145-000/43980","Digikey")</f>
@@ -16973,13 +16943,13 @@
     </row>
     <row r="26" spans="1:11" ht="50.1" customHeight="1">
       <c r="A26" s="34" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C26" s="31">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="5">
@@ -16991,19 +16961,19 @@
         <v>20.596529999999998</v>
       </c>
       <c r="H26" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K26" s="32"/>
     </row>
     <row r="27" spans="1:11" ht="50.1" customHeight="1">
       <c r="A27" s="31" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C27" s="31">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E27" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A207/", "McMaster")</f>
@@ -17018,19 +16988,19 @@
         <v>2.9393999999999996</v>
       </c>
       <c r="H27" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K27" s="32"/>
     </row>
     <row r="28" spans="1:11" ht="50.1" customHeight="1">
       <c r="A28" s="31" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C28" s="31">
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E28" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A210/", "McMaster")</f>
@@ -17045,19 +17015,19 @@
         <v>1.6015999999999999</v>
       </c>
       <c r="H28" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K28" s="32"/>
     </row>
     <row r="29" spans="1:11" ht="50.1" customHeight="1">
       <c r="A29" s="31" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C29" s="31">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E29" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A216/", "McMaster")</f>
@@ -17072,19 +17042,19 @@
         <v>0.30559999999999998</v>
       </c>
       <c r="H29" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11" ht="50.1" customHeight="1">
       <c r="A30" s="31" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C30" s="31">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E30" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/94500A227/", "McMaster")</f>
@@ -17099,18 +17069,18 @@
         <v>0.61599999999999999</v>
       </c>
       <c r="H30" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="50.1" customHeight="1">
       <c r="A31" s="31" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C31" s="31">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E31" s="32" t="str">
         <f t="shared" ref="E31" si="4">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -17125,22 +17095,22 @@
         <v>0.94950000000000001</v>
       </c>
       <c r="H31" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K31" s="32"/>
     </row>
     <row r="32" spans="1:11" ht="50.1" customHeight="1">
       <c r="A32" s="31" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C32" s="31">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E32" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A208/", "McMaster")</f>
@@ -17155,13 +17125,13 @@
         <v>0.65319999999999989</v>
       </c>
       <c r="H32" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I32" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K32" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3I9bwDb", "Amazon")</f>
@@ -17170,13 +17140,13 @@
     </row>
     <row r="33" spans="1:11" ht="50.1" customHeight="1">
       <c r="A33" s="31" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C33" s="31">
         <v>19</v>
       </c>
       <c r="D33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E33" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3I8VKIx", "Amazon")</f>
@@ -17191,13 +17161,13 @@
         <v>4.1761999999999997</v>
       </c>
       <c r="H33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I33" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J33" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K33" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90510A232/", "McMaster")</f>
@@ -17206,13 +17176,13 @@
     </row>
     <row r="34" spans="1:11" ht="50.1" customHeight="1">
       <c r="A34" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C34" s="31">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E34" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90591A260/", "McMaster")</f>
@@ -17227,10 +17197,10 @@
         <v>3.56E-2</v>
       </c>
       <c r="H34" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I34" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K34" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3v5pm5K", "Amazon")</f>
@@ -17239,16 +17209,16 @@
     </row>
     <row r="35" spans="1:11" ht="50.1" customHeight="1">
       <c r="A35" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B35" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E35" s="32" t="str">
         <f>HYPERLINK("https://shop.polybelt.com/650-5m-09-Urethane-Steel-Timing-Belt-130-Tooth-B650-5M-09CPS.htm", "PolyBelt")</f>
@@ -17262,7 +17232,7 @@
         <v>13.5</v>
       </c>
       <c r="H35" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K35" s="32"/>
     </row>
@@ -17990,7 +17960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CADD61D-F9D2-4804-993E-5F65E31FCDDD}">
   <dimension ref="A1:AF23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -18032,7 +18002,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -18067,19 +18037,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -18091,27 +18061,27 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C3" s="34">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="5">
         <f>'Electrical '!I52</f>
@@ -18122,7 +18092,7 @@
         <v>34.43</v>
       </c>
       <c r="H3" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="7">
@@ -18132,13 +18102,13 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="34" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C4" s="34">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E4" s="32" t="str">
         <f>HYPERLINK("https://developer.nvidia.com/embedded/jetson-nano-2gb-developer-kit","Nvidia")</f>
@@ -18155,13 +18125,13 @@
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="34" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C5" s="34">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3t85BIe","Amazon")</f>
@@ -18179,13 +18149,13 @@
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="34" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C6" s="34">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E6" s="32" t="str">
         <f>HYPERLINK("https://bit.ly/3pgw6dg","Seahorse")</f>
@@ -18202,13 +18172,13 @@
     </row>
     <row r="7" spans="1:32" ht="50.1" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C7" s="34">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3JW5hmK","Amazon")</f>
@@ -18226,13 +18196,13 @@
     </row>
     <row r="8" spans="1:32" ht="50.1" customHeight="1">
       <c r="A8" s="34" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C8" s="34">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E8" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3JNUvPk", "Amazon")</f>
@@ -18249,13 +18219,13 @@
     </row>
     <row r="9" spans="1:32" ht="50.1" customHeight="1">
       <c r="A9" s="34" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C9" s="34">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E9" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -18270,19 +18240,19 @@
         <v>0.53171999999999997</v>
       </c>
       <c r="H9" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:32" ht="50.1" customHeight="1">
       <c r="A10" s="34" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C10" s="34">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E10" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3M5yQ72", "Amazon")</f>
@@ -18300,13 +18270,13 @@
     </row>
     <row r="11" spans="1:32" ht="50.1" customHeight="1">
       <c r="A11" s="34" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C11" s="34">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E11" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/35rtwKr", "Amazon")</f>
@@ -18323,13 +18293,13 @@
     </row>
     <row r="12" spans="1:32" ht="50.1" customHeight="1">
       <c r="A12" s="34" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C12" s="34">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E12" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -18344,25 +18314,25 @@
         <v>0.51273000000000002</v>
       </c>
       <c r="H12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K12" s="32"/>
     </row>
     <row r="13" spans="1:32" ht="50.1" customHeight="1">
       <c r="A13" s="34" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C13" s="34">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E13" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/35x7YMk","Amazon")</f>
@@ -18380,13 +18350,13 @@
     </row>
     <row r="14" spans="1:32" ht="50.1" customHeight="1">
       <c r="A14" s="34" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C14" s="34">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E14" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/359tuHm", "Amazon")</f>
@@ -18404,13 +18374,13 @@
     </row>
     <row r="15" spans="1:32" ht="50.1" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C15" s="34">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E15" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3HoIvlN", "Amazon")</f>
@@ -18428,13 +18398,13 @@
     </row>
     <row r="16" spans="1:32" ht="50.1" customHeight="1">
       <c r="A16" s="34" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C16" s="34">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E16" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -18449,19 +18419,19 @@
         <v>0.81657000000000002</v>
       </c>
       <c r="H16" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:11" ht="50.1" customHeight="1">
       <c r="A17" s="34" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C17" s="34">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E17" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -18476,19 +18446,19 @@
         <v>0.81657000000000002</v>
       </c>
       <c r="H17" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="50.1" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C18" s="34">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E18" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/94500A223/", "McMaster")</f>
@@ -18506,13 +18476,13 @@
     </row>
     <row r="19" spans="1:11" ht="50.1" customHeight="1">
       <c r="A19" s="34" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C19" s="34">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E19" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3pifPEE", "Amazon")</f>
@@ -18530,13 +18500,13 @@
     </row>
     <row r="20" spans="1:11" ht="50.1" customHeight="1">
       <c r="A20" s="34" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C20" s="34">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E20" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -18551,19 +18521,19 @@
         <v>1.02546</v>
       </c>
       <c r="H20" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K20" s="32"/>
     </row>
     <row r="21" spans="1:11" ht="50.1" customHeight="1">
       <c r="A21" s="34" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C21" s="34">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E21" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3slfva4", "Amazon")</f>
@@ -18581,13 +18551,13 @@
     </row>
     <row r="22" spans="1:11" ht="50.1" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C22" s="34">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E22" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A216/", "McMaster")</f>
@@ -18602,19 +18572,19 @@
         <v>0.61119999999999997</v>
       </c>
       <c r="H22" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K22" s="32"/>
     </row>
     <row r="23" spans="1:11" ht="50.1" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C23" s="34">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E23" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A208/", "McMaster")</f>
@@ -18629,13 +18599,13 @@
         <v>0.97979999999999978</v>
       </c>
       <c r="H23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K23" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3I9bwDb", "Amazon")</f>
@@ -19265,7 +19235,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -19300,19 +19270,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -19324,28 +19294,28 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="31" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C3" s="31">
         <f>Overall!N9+1</f>
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="5">
@@ -19357,7 +19327,7 @@
         <v>60.720000000000006</v>
       </c>
       <c r="H3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="7">
@@ -19367,13 +19337,13 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="31" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C4" s="31">
         <v>1</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E4" s="32" t="str">
         <f t="shared" ref="E4" si="0">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -19388,23 +19358,23 @@
         <v>0.30384</v>
       </c>
       <c r="H4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="31" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C5" s="31">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E5" s="32" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/littelfuse-inc/59145-040/4771993","Digikey")</f>
@@ -19418,19 +19388,19 @@
         <v>4.95</v>
       </c>
       <c r="H5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C6" s="31">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E6" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3pcFWwW", "Amazon")</f>
@@ -19445,13 +19415,13 @@
         <v>3.3979999999999997</v>
       </c>
       <c r="H6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K6" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/35ijWtt", "Amazon")</f>
@@ -19460,13 +19430,13 @@
     </row>
     <row r="7" spans="1:32" ht="50.1" customHeight="1">
       <c r="A7" s="31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C7" s="31">
         <v>10</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="32" t="str">
         <f t="shared" ref="E7" si="1">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -19481,10 +19451,10 @@
         <v>2.4687000000000001</v>
       </c>
       <c r="H7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J7" s="32"/>
       <c r="K7" s="32" t="str">
@@ -19494,13 +19464,13 @@
     </row>
     <row r="8" spans="1:32" ht="50.1" customHeight="1">
       <c r="A8" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C8" s="31">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="5">
@@ -19608,7 +19578,7 @@
     </row>
     <row r="22" spans="1:11" ht="50.1" customHeight="1">
       <c r="A22" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -19807,7 +19777,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6 F3">
+  <conditionalFormatting sqref="F3 F6">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -20089,7 +20059,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -20124,19 +20094,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -20148,21 +20118,21 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="31" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C3" s="31">
         <v>1</v>
@@ -20183,13 +20153,13 @@
         <v>4.7449999999999992</v>
       </c>
       <c r="H3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K3" s="32" t="str">
         <f>HYPERLINK("https://www.amazon.com/Aluminum-Extrusion-European-Standard-Anodized/dp/B08CN92SP1/ref=sr_1_7?crid=3VIGODRUEW0NZ&amp;keywords=150mm+2040&amp;qid=1645476496&amp;sprefix=150mm+2040%2Caps%2C147&amp;sr=8-7", "Amazon")</f>
@@ -20202,7 +20172,7 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="31" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C4" s="31">
         <v>4</v>
@@ -20222,13 +20192,13 @@
         <v>7.76</v>
       </c>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K4" s="32" t="str">
         <f>HYPERLINK("https://www.amazon.com/Aluminum-Extrusion-Corner-Bracket-Profile/dp/B08N16BKQS/ref=sr_1_7?crid=2K2OD6C5WR7GM&amp;keywords=right+angle+8020&amp;qid=1645476638&amp;sprefix=right+angle+8020%2Caps%2C149&amp;sr=8-7", "Amazon")</f>
@@ -20237,13 +20207,13 @@
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="31" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C5" s="31">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="5">
@@ -20255,22 +20225,22 @@
         <v>4.7893800000000004</v>
       </c>
       <c r="H5" t="s">
+        <v>276</v>
+      </c>
+      <c r="I5" t="s">
         <v>278</v>
-      </c>
-      <c r="I5" t="s">
-        <v>280</v>
       </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C6" s="31">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E6" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -20285,16 +20255,16 @@
         <v>0.48</v>
       </c>
       <c r="H6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:32" ht="50.1" customHeight="1">
       <c r="A7" s="34" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C7" s="31">
         <v>3</v>
@@ -20315,10 +20285,10 @@
         <v>20.939999999999998</v>
       </c>
       <c r="H7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K7" s="32" t="str">
         <f>HYPERLINK("https://www.amazon.com/European-Standard-Anodized-Aluminum-Extrusion/dp/B099N9QCTJ/ref=sr_1_4?crid=WNRTCAE6OMWK&amp;keywords=2040+300mm&amp;qid=1645478233&amp;sprefix=2040+300mm%2Caps%2C190&amp;sr=8-4", "Amazon")</f>
@@ -20327,13 +20297,13 @@
     </row>
     <row r="8" spans="1:32" ht="50.1" customHeight="1">
       <c r="A8" s="31" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C8" s="31">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E8" s="32" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/970300581/6174852", "DigiKey")</f>
@@ -20347,7 +20317,7 @@
         <v>3.04</v>
       </c>
       <c r="H8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K8" s="32" t="str">
         <f t="shared" ref="K8:K15" si="1">HYPERLINK("", "Amazon")</f>
@@ -20356,13 +20326,13 @@
     </row>
     <row r="9" spans="1:32" ht="50.1" customHeight="1">
       <c r="A9" s="31" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C9" s="31">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="5">
@@ -20374,10 +20344,10 @@
         <v>4.7893800000000004</v>
       </c>
       <c r="H9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="K9" s="32" t="str">
         <f t="shared" si="1"/>
@@ -20386,13 +20356,13 @@
     </row>
     <row r="10" spans="1:32" ht="50.1" customHeight="1">
       <c r="A10" s="31" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C10" s="31">
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E10" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A208/", "McMaster")</f>
@@ -20407,13 +20377,13 @@
         <v>5.8787999999999991</v>
       </c>
       <c r="H10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K10" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3I9bwDb", "Amazon")</f>
@@ -20422,13 +20392,13 @@
     </row>
     <row r="11" spans="1:32" ht="50.1" customHeight="1">
       <c r="A11" s="31" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C11" s="31">
         <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E11" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3I8VKIx", "Amazon")</f>
@@ -20443,13 +20413,13 @@
         <v>8.7919999999999998</v>
       </c>
       <c r="H11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K11" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90510A232/", "McMaster")</f>
@@ -20458,13 +20428,13 @@
     </row>
     <row r="12" spans="1:32" ht="50.1" customHeight="1">
       <c r="A12" s="31" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C12" s="31">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E12" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/5537T425/", "McMaster")</f>
@@ -20479,13 +20449,13 @@
         <v>3.5150000000000001</v>
       </c>
       <c r="H12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K12" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3s5sT1T", "Amazon")</f>
@@ -20494,13 +20464,13 @@
     </row>
     <row r="13" spans="1:32" ht="50.1" customHeight="1">
       <c r="A13" s="31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C13" s="31">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="5">
@@ -20512,7 +20482,7 @@
         <v>14.721939999999998</v>
       </c>
       <c r="H13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K13" s="32" t="str">
         <f t="shared" si="1"/>
@@ -20521,13 +20491,13 @@
     </row>
     <row r="14" spans="1:32" ht="50.1" customHeight="1">
       <c r="A14" s="34" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C14" s="31">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="5">
@@ -20539,7 +20509,7 @@
         <v>13.00104</v>
       </c>
       <c r="H14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K14" s="32" t="str">
         <f t="shared" si="1"/>
@@ -20548,13 +20518,13 @@
     </row>
     <row r="15" spans="1:32" ht="50.1" customHeight="1">
       <c r="A15" s="31" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C15" s="31">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="5">
@@ -20566,7 +20536,7 @@
         <v>14.721939999999998</v>
       </c>
       <c r="H15" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K15" s="32" t="str">
         <f t="shared" si="1"/>
@@ -20575,13 +20545,13 @@
     </row>
     <row r="16" spans="1:32" ht="50.1" customHeight="1">
       <c r="A16" s="31" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C16" s="31">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E16" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A210/", "McMaster")</f>
@@ -20596,10 +20566,10 @@
         <v>0.80079999999999996</v>
       </c>
       <c r="H16" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I16" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="K16" s="32"/>
     </row>
@@ -20792,7 +20762,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -20827,19 +20797,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -20851,27 +20821,27 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="31" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C3" s="31">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E3" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/5537T425/", "McMaster")</f>
@@ -20886,13 +20856,13 @@
         <v>7.03</v>
       </c>
       <c r="H3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K3" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3s5sT1T", "Amazon")</f>
@@ -20905,7 +20875,7 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="31" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C4" s="31">
         <v>1</v>
@@ -20926,10 +20896,10 @@
         <v>53.690000000000005</v>
       </c>
       <c r="H4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K4" s="32"/>
     </row>
@@ -21060,7 +21030,7 @@
     </row>
     <row r="22" spans="1:11" ht="50.1" customHeight="1">
       <c r="A22" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -21505,7 +21475,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -21540,19 +21510,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -21564,27 +21534,27 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="31" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C3" s="31">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3JJ8RAm", "Amazon")</f>
@@ -21599,7 +21569,7 @@
         <v>1.5960000000000001</v>
       </c>
       <c r="H3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="7">
@@ -21609,13 +21579,13 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="31" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C4" s="31">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E4" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A187/", "McMaster")</f>
@@ -21630,22 +21600,22 @@
         <v>0.28520000000000001</v>
       </c>
       <c r="H4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="31" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C5" s="31">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3v8bl7r","Amazon")</f>
@@ -21663,13 +21633,13 @@
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C6" s="31">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="5">
@@ -21684,13 +21654,13 @@
     </row>
     <row r="7" spans="1:32" ht="50.1" customHeight="1">
       <c r="A7" s="31" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C7" s="31">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="5"/>
@@ -21702,13 +21672,13 @@
     </row>
     <row r="8" spans="1:32" ht="50.1" customHeight="1">
       <c r="A8" s="31" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C8" s="31">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="5">
@@ -21723,13 +21693,13 @@
     </row>
     <row r="9" spans="1:32" ht="50.1" customHeight="1">
       <c r="A9" s="31" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C9" s="31">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="5">
@@ -21744,13 +21714,13 @@
     </row>
     <row r="10" spans="1:32" ht="50.1" customHeight="1">
       <c r="A10" s="31" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C10" s="31">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="5">
@@ -21765,7 +21735,7 @@
     </row>
     <row r="11" spans="1:32" ht="50.1" customHeight="1">
       <c r="A11" s="31" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C11" s="31">
         <v>2</v>
@@ -21786,13 +21756,13 @@
         <v>10.98</v>
       </c>
       <c r="H11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K11" s="32" t="str">
         <f>HYPERLINK("https://www.amazon.com/Aluminum-Extrusion-European-Standard-Anodized/dp/B08CN92SP1/ref=sr_1_7?crid=3VIGODRUEW0NZ&amp;keywords=150mm+2040&amp;qid=1645476496&amp;sprefix=150mm+2040%2Caps%2C147&amp;sr=8-7", "Amazon")</f>
@@ -21801,13 +21771,13 @@
     </row>
     <row r="12" spans="1:32" ht="50.1" customHeight="1">
       <c r="A12" s="31" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C12" s="31">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="5">
@@ -21822,13 +21792,13 @@
     </row>
     <row r="13" spans="1:32" ht="50.1" customHeight="1">
       <c r="A13" s="31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C13" s="31">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="5">
@@ -21843,13 +21813,13 @@
     </row>
     <row r="14" spans="1:32" ht="50.1" customHeight="1">
       <c r="A14" s="31" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C14" s="31">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E14" s="32" t="str">
         <f>HYPERLINK("https://www.amazon.com/gp/product/B07CXNK33Q/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1","Amazon")</f>
@@ -21863,22 +21833,22 @@
         <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:32" ht="50.1" customHeight="1">
       <c r="A15" s="34" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C15" s="31">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E15" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/95947A725/", "Amazon")</f>
@@ -21895,13 +21865,13 @@
     </row>
     <row r="16" spans="1:32" ht="50.1" customHeight="1">
       <c r="A16" s="31" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C16" s="31">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E16" s="32" t="str">
         <f>HYPERLINK("https://bit.ly/3t0jHvb", "StepperOnline")</f>
@@ -21918,13 +21888,13 @@
     </row>
     <row r="17" spans="1:11" ht="50.1" customHeight="1">
       <c r="A17" s="31" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C17" s="31">
         <v>1</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E17" s="32" t="str">
         <f t="shared" ref="E17:E18" si="0">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -21939,23 +21909,23 @@
         <v>2.1268799999999999</v>
       </c>
       <c r="H17" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="50.1" customHeight="1">
       <c r="A18" s="31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C18" s="31">
         <v>2</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E18" s="32" t="str">
         <f t="shared" si="0"/>
@@ -21970,23 +21940,23 @@
         <v>0.53171999999999997</v>
       </c>
       <c r="H18" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="I18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="50.1" customHeight="1">
       <c r="A19" s="31" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C19" s="31">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E19" s="32" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/littelfuse-inc/57145-000/43980","Digikey")</f>
@@ -22000,19 +21970,19 @@
         <v>3.06</v>
       </c>
       <c r="H19" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" ht="50.1" customHeight="1">
       <c r="A20" s="31" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C20" s="31">
         <v>1</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E20" s="32" t="str">
         <f t="shared" ref="E20:E24" si="1">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -22027,23 +21997,23 @@
         <v>0.20888999999999999</v>
       </c>
       <c r="H20" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
     <row r="21" spans="1:11" ht="50.1" customHeight="1">
       <c r="A21" s="31" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C21" s="31">
         <v>1</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E21" s="32" t="str">
         <f t="shared" si="1"/>
@@ -22058,23 +22028,23 @@
         <v>0.32283000000000001</v>
       </c>
       <c r="H21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
     <row r="22" spans="1:11" ht="50.1" customHeight="1">
       <c r="A22" s="31" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C22" s="31">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="5">
@@ -22089,13 +22059,13 @@
     </row>
     <row r="23" spans="1:11" ht="50.1" customHeight="1">
       <c r="A23" s="31" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C23" s="31">
         <v>1</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E23" s="32" t="str">
         <f t="shared" si="1"/>
@@ -22110,23 +22080,23 @@
         <v>2.0509200000000001</v>
       </c>
       <c r="H23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:11" ht="50.1" customHeight="1">
       <c r="A24" s="31" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C24" s="31">
         <v>2</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E24" s="32" t="str">
         <f t="shared" si="1"/>
@@ -22141,23 +22111,23 @@
         <v>0.26585999999999999</v>
       </c>
       <c r="H24" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" ht="50.1" customHeight="1">
       <c r="A25" s="31" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C25" s="31">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E25" s="32" t="str">
         <f>HYPERLINK("https://www.ebay.com/itm/392938210815", "Ebay")</f>
@@ -22177,7 +22147,7 @@
     </row>
     <row r="26" spans="1:11" ht="50.1" customHeight="1">
       <c r="A26" s="31" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C26" s="31">
         <v>1</v>
@@ -22194,7 +22164,7 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="K26" s="32" t="str">
         <f t="shared" si="2"/>
@@ -22203,7 +22173,7 @@
     </row>
     <row r="27" spans="1:11" ht="50.1" customHeight="1">
       <c r="A27" s="31" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C27" s="31">
         <v>1</v>
@@ -22220,7 +22190,7 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="K27" s="32" t="str">
         <f t="shared" si="2"/>
@@ -22229,13 +22199,13 @@
     </row>
     <row r="28" spans="1:11" ht="50.1" customHeight="1">
       <c r="A28" s="31" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C28" s="31">
         <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E28" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3I8VKIx", "Amazon")</f>
@@ -22250,13 +22220,13 @@
         <v>7.0335999999999999</v>
       </c>
       <c r="H28" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I28" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K28" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90510A232/", "McMaster")</f>
@@ -22265,13 +22235,13 @@
     </row>
     <row r="29" spans="1:11" ht="50.1" customHeight="1">
       <c r="A29" s="31" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C29" s="31">
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E29" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A208/", "McMaster")</f>
@@ -22286,13 +22256,13 @@
         <v>4.8989999999999991</v>
       </c>
       <c r="H29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K29" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3I9bwDb", "Amazon")</f>
@@ -22301,13 +22271,13 @@
     </row>
     <row r="30" spans="1:11" ht="50.1" customHeight="1">
       <c r="A30" s="31" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C30" s="31">
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E30" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A216/", "McMaster")</f>
@@ -22322,19 +22292,19 @@
         <v>0.61119999999999997</v>
       </c>
       <c r="H30" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K30" s="32"/>
     </row>
     <row r="31" spans="1:11" ht="50.1" customHeight="1">
       <c r="A31" s="31" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C31" s="31">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E31" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A218/", "McMaster")</f>
@@ -22355,13 +22325,13 @@
     </row>
     <row r="32" spans="1:11" ht="50.1" customHeight="1">
       <c r="A32" s="31" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C32" s="31">
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E32" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A214/", "McMaster")</f>
@@ -22382,13 +22352,13 @@
     </row>
     <row r="33" spans="1:11" ht="50.1" customHeight="1">
       <c r="A33" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C33" s="31">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E33" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90591A260/", "McMaster")</f>
@@ -22403,10 +22373,10 @@
         <v>0.1424</v>
       </c>
       <c r="H33" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I33" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K33" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3v5pm5K", "Amazon")</f>
@@ -22415,13 +22385,13 @@
     </row>
     <row r="34" spans="1:11" ht="50.1" customHeight="1">
       <c r="A34" s="31" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C34" s="31">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E34" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/92095A475/", "McMaster")</f>
@@ -22436,22 +22406,22 @@
         <v>0.64</v>
       </c>
       <c r="H34" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I34" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K34" s="32"/>
     </row>
     <row r="35" spans="1:11" ht="50.1" customHeight="1">
       <c r="A35" s="31" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C35" s="31">
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E35" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3JSYdHx", "Amazon")</f>
@@ -22466,7 +22436,7 @@
         <v>0.26970000000000005</v>
       </c>
       <c r="H35" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="K35" s="32"/>
     </row>
@@ -23548,7 +23518,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="50.1" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -23583,19 +23553,19 @@
     </row>
     <row r="2" spans="1:32" ht="50.1" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>243</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>7</v>
@@ -23607,27 +23577,27 @@
         <v>11</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="50.1" customHeight="1">
       <c r="A3" s="31" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C3" s="31">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3pcU6xT", "Amazon")</f>
@@ -23642,7 +23612,7 @@
         <v>1.599</v>
       </c>
       <c r="H3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="7">
@@ -23652,13 +23622,13 @@
     </row>
     <row r="4" spans="1:32" ht="50.1" customHeight="1">
       <c r="A4" s="31" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C4" s="31">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E4" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/91306A736/", "McMaster")</f>
@@ -23673,13 +23643,13 @@
         <v>0.55120000000000002</v>
       </c>
       <c r="H4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K4" s="32" t="str">
         <f>HYPERLINK("https://www.amazon.com/ZAYI-M5-0-8-Stainless-Finish%EF%BC%8CMetric-Fastener/dp/B09MRGZ473/ref=sr_1_3?crid=3FJWNU9KFFIX0&amp;keywords=M5+50mm&amp;qid=1645477676&amp;sprefix=m5+50mm%2Caps%2C146&amp;sr=8-3", "Amazon")</f>
@@ -23688,13 +23658,13 @@
     </row>
     <row r="5" spans="1:32" ht="50.1" customHeight="1">
       <c r="A5" s="31" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C5" s="31">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -23708,22 +23678,22 @@
         <v>1.899E-2</v>
       </c>
       <c r="H5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:32" ht="50.1" customHeight="1">
       <c r="A6" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C6" s="31">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E6" s="32" t="str">
         <f t="shared" ref="E6:E7" si="0">HYPERLINK("https://amzn.to/3p4Z7Zp", "PETG")</f>
@@ -23737,22 +23707,22 @@
         <v>1.899E-2</v>
       </c>
       <c r="H6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:32" ht="50.1" customHeight="1">
       <c r="A7" s="31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C7" s="31">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="32" t="str">
         <f t="shared" si="0"/>
@@ -23767,22 +23737,22 @@
         <v>0.17091000000000001</v>
       </c>
       <c r="H7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:32" ht="50.1" customHeight="1">
       <c r="A8" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C8" s="31">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E8" s="32" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/90591A260/", "McMaster")</f>
@@ -23797,10 +23767,10 @@
         <v>3.56E-2</v>
       </c>
       <c r="H8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K8" s="32" t="str">
         <f>HYPERLINK("https://amzn.to/3v5pm5K", "Amazon")</f>

</xml_diff>